<commit_message>
_ Updated version of the Industry_model_final.py   * All issues were solved   * Emissions optimization is now possible   * In the case of negative emissions, cost variable will not diminish with carbon tax _ Steel industry case study (see Steel_scenarios.py that can be found here: https://www.overleaf.com/read/chsvfsqsncjf
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Steel/Data/v2/Steel_Technologies.xlsx
+++ b/Models/Industry_model/Input/Steel/Data/v2/Steel_Technologies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q.raillard-cazanove\ownCloud\1ère année\Optim modelling\Project\Etude_TP_CapaExpPlaning-Python\Models\Industry_model\Input\Steel\Data\v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6667E7-419C-481F-A3A3-C10FF7F1B559}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B4A7D0-F843-4FF7-B0D2-C7131AA11BF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
   <si>
     <t>coal</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>discount_rate</t>
+  </si>
+  <si>
+    <t>CCS</t>
+  </si>
+  <si>
+    <t>https://www.globalccsinstitute.com/wp-content/uploads/2021/03/Technology-Readiness-and-Costs-for-CCS-2021-1.pdf</t>
+  </si>
+  <si>
+    <t>(Kearns et al, 2021)</t>
   </si>
 </sst>
 </file>
@@ -259,7 +268,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +323,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -352,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -390,12 +405,32 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -745,21 +780,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{013CB58D-7F5B-4EF4-A405-5ECDD25301A7}" name="Tableau3" displayName="Tableau3" ref="A1:L19" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A1:L19" xr:uid="{87FB60C7-DCAA-43CC-AAD9-BB44B0181513}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{42A5F6EE-6AFE-476D-8B1C-92974D7ECF5E}" name="Resource" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{9D816E12-F9ED-4134-84FD-E84CE7055F94}" name="unit" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{DB97F9EF-90E4-4C9C-991F-8DAD126D2235}" name="Scrap" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{E1370907-462D-42E0-BEE5-5C402344A846}" name="Pellet_making" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{9C579E2B-EFB9-4CDF-90A8-B8E4B9421C12}" name="BF-BOF" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{B0DEE251-5BB2-4367-BFBD-103A29B0561A}" name="H2-BF-BOF" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{2E6C1B91-C3DE-4354-BCF7-60140C2C1CA3}" name="BioBF-BOF" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{559435F3-4582-467F-8C76-B10399D7D78A}" name="EAF" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{E1E290F6-88F7-451F-9364-C275A967D90D}" name="H-DRI-EAF" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{1F484475-C8B0-425E-87D5-19B30AEACB25}" name="CH4-DRI-EAF" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{D0015D03-4CF5-4EF1-9804-DE585190B1D4}" name="BioDRI-EAF" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{7F11CCD2-8961-4412-87AE-60BC0FD4F71A}" name="Coal-DRI-EAF" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{013CB58D-7F5B-4EF4-A405-5ECDD25301A7}" name="Tableau3" displayName="Tableau3" ref="A1:M19" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="A1:M19" xr:uid="{87FB60C7-DCAA-43CC-AAD9-BB44B0181513}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{42A5F6EE-6AFE-476D-8B1C-92974D7ECF5E}" name="Resource" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{9D816E12-F9ED-4134-84FD-E84CE7055F94}" name="unit" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{DB97F9EF-90E4-4C9C-991F-8DAD126D2235}" name="Scrap" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{E1370907-462D-42E0-BEE5-5C402344A846}" name="Pellet_making" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{9C579E2B-EFB9-4CDF-90A8-B8E4B9421C12}" name="BF-BOF" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{B0DEE251-5BB2-4367-BFBD-103A29B0561A}" name="H2-BF-BOF" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{2E6C1B91-C3DE-4354-BCF7-60140C2C1CA3}" name="BioBF-BOF" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{559435F3-4582-467F-8C76-B10399D7D78A}" name="EAF" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{E1E290F6-88F7-451F-9364-C275A967D90D}" name="H-DRI-EAF" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{1F484475-C8B0-425E-87D5-19B30AEACB25}" name="CH4-DRI-EAF" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{D0015D03-4CF5-4EF1-9804-DE585190B1D4}" name="BioDRI-EAF" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{7F11CCD2-8961-4412-87AE-60BC0FD4F71A}" name="Coal-DRI-EAF" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{2411BD64-AE68-4907-BEB4-476FC7533970}" name="CCS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1074,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0CEE37-33A3-4179-A627-9FAA023AC5EF}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1122,7 @@
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -1123,8 +1159,11 @@
       <c r="L1" s="8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1157,8 +1196,9 @@
       <c r="L2" s="9">
         <v>-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>49</v>
       </c>
@@ -1191,8 +1231,9 @@
       <c r="L3" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>25</v>
       </c>
@@ -1213,8 +1254,9 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1236,8 +1278,9 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1284,8 +1327,9 @@
         <f>Tableau3[[#This Row],[H-DRI-EAF]]</f>
         <v>1.6199870401036789E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
@@ -1314,8 +1358,9 @@
         <f>0.853/'Conversion table'!B4</f>
         <v>0.12848432777391336</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -1338,8 +1383,9 @@
         <v>0.19192346461228307</v>
       </c>
       <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
@@ -1356,8 +1402,9 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1374,8 +1421,9 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -1421,8 +1469,9 @@
         <f>0.38+0.753+Tableau3[[#This Row],[BF-BOF]]</f>
         <v>1.327</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
@@ -1439,8 +1488,11 @@
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1478,8 +1530,9 @@
         <f>1.048+0.307</f>
         <v>1.355</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
@@ -1520,8 +1573,9 @@
         <f t="shared" si="2"/>
         <v>414</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>57</v>
       </c>
@@ -1554,8 +1608,9 @@
       <c r="L15" s="22">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>60</v>
       </c>
@@ -1586,8 +1641,9 @@
       <c r="L16" s="23">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>59</v>
       </c>
@@ -1626,8 +1682,9 @@
         <f t="shared" si="3"/>
         <v>0.11745962477254576</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="9"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
@@ -1664,8 +1721,11 @@
       <c r="L18" s="27">
         <v>53.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>12</v>
       </c>
@@ -1708,6 +1768,7 @@
         <f>1.048</f>
         <v>1.048</v>
       </c>
+      <c r="M19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1786,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1196D17-6166-40A9-953F-A236C50591E1}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:C10"/>
+      <selection activeCell="A14" sqref="A14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,6 +1970,17 @@
       </c>
       <c r="C13" s="21" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>